<commit_message>
running our tests in a factory
</commit_message>
<xml_diff>
--- a/src/test/resources/tests_excels/feeTypeTestCases.xlsx
+++ b/src/test/resources/tests_excels/feeTypeTestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865"/>
   </bookViews>
   <sheets>
     <sheet name="test cases" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,6 @@
     <t>code</t>
   </si>
   <si>
-    <t>Kazakhstan Country</t>
-  </si>
-  <si>
-    <t>KZC</t>
-  </si>
-  <si>
-    <t>USA Country</t>
-  </si>
-  <si>
     <t>already exists</t>
   </si>
   <si>
@@ -89,6 +80,15 @@
   </si>
   <si>
     <t>apiPath</t>
+  </si>
+  <si>
+    <t>Kazakhstan FEE</t>
+  </si>
+  <si>
+    <t>KZF</t>
+  </si>
+  <si>
+    <t>USA FEE</t>
   </si>
 </sst>
 </file>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -960,13 +960,13 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>0</v>
@@ -977,10 +977,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>26345345</v>
@@ -989,7 +989,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" s="5">
         <v>201</v>
@@ -1001,7 +1001,7 @@
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
         <v>26345345</v>
@@ -1010,21 +1010,21 @@
         <v>101</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" s="5">
         <v>400</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <v>26345345</v>
@@ -1033,13 +1033,13 @@
         <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="5">
         <v>400</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1052,18 +1052,18 @@
         <v>103</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F5" s="5">
         <v>400</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -1073,13 +1073,13 @@
         <v>104</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" s="5">
         <v>400</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1103,34 +1103,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="21">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>